<commit_message>
Atualização do Boletim de Acompanhamento e Relatório Mensal de Pagamentos das OS - Ref. a Set/2016.
</commit_message>
<xml_diff>
--- a/00_GESTAO_GERAL/00_COMITE/04_RELATORIO_MENSAL/Relatóro Mensal de Ordens de Serviços - 201609.xlsx
+++ b/00_GESTAO_GERAL/00_COMITE/04_RELATORIO_MENSAL/Relatóro Mensal de Ordens de Serviços - 201609.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositorio\Sistema\00_GESTAO_GERAL\00_COMITE\04_RELATORIO_MENSAL\"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="212">
   <si>
     <t>Número OS</t>
   </si>
@@ -702,10 +702,10 @@
     <t>PF Alterado</t>
   </si>
   <si>
-    <t>Correção</t>
-  </si>
-  <si>
     <t>Do Mês</t>
+  </si>
+  <si>
+    <t>Recebida_</t>
   </si>
 </sst>
 </file>
@@ -3035,6 +3035,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3197,6 +3198,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Planilha10"/>
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -4158,6 +4160,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Planilha11"/>
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4192,9 +4195,9 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="71">
+      <c r="A2" s="71" t="str">
         <f ca="1">IF(FatCTL[[#This Row],[Número OS]]="","",IF(FatCTL[[#This Row],[0]]=E1,"",FatCTL[[#This Row],[0]]))</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="B2" s="68">
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($B$1)-1))+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($B$1)-1))+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($B$1)-1))+1,OSCTL[],2,FALSE),""))</f>
@@ -4202,21 +4205,21 @@
       </c>
       <c r="C2" s="77">
         <f ca="1">IF(FatCTL[[#This Row],[Número OS]]="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(FatCTL[[#This Row],[Número OS]],Mensal!$A$5:$A$154,0)+1,4)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(FatCTL[[#This Row],[Número OS]],Mensal!$A$5:$A$154,0)+1,4)))</f>
-        <v>216.8</v>
+        <v>0</v>
       </c>
       <c r="D2" s="77">
         <f ca="1">IF(B2="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B2,Mensal!$A$5:$A$154,0)+4,3)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B2,Mensal!$A$5:$A$154,0)+4,3)))</f>
-        <v>162.60000000000002</v>
-      </c>
-      <c r="E2" s="70">
+        <v>0</v>
+      </c>
+      <c r="E2" s="70" t="str">
         <f ca="1">IF(FatCTL[[#This Row],[Saldo em PF]]=0,E1,E1+1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="71">
         <f ca="1">IF(FatCTL[[#This Row],[Número OS]]="","",IF(FatCTL[[#This Row],[0]]=E2,"",FatCTL[[#This Row],[0]]))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="68">
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($B$1)-1))+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($B$1)-1))+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($B$1)-1))+1,OSCTL[],2,FALSE),""))</f>
@@ -4232,13 +4235,13 @@
       </c>
       <c r="E3" s="70">
         <f ca="1">IF(FatCTL[[#This Row],[Saldo em PF]]=0,E2,E2+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="71">
         <f ca="1">IF(FatCTL[[#This Row],[Número OS]]="","",IF(FatCTL[[#This Row],[0]]=E3,"",FatCTL[[#This Row],[0]]))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="68">
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($B$1)-1))+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($B$1)-1))+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($B$1)-1))+1,OSCTL[],2,FALSE),""))</f>
@@ -4254,13 +4257,13 @@
       </c>
       <c r="E4" s="70">
         <f ca="1">IF(FatCTL[[#This Row],[Saldo em PF]]=0,E3,E3+1)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="71">
         <f ca="1">IF(FatCTL[[#This Row],[Número OS]]="","",IF(FatCTL[[#This Row],[0]]=E4,"",FatCTL[[#This Row],[0]]))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="68">
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($B$1)-1))+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($B$1)-1))+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($B$1)-1))+1,OSCTL[],2,FALSE),""))</f>
@@ -4276,13 +4279,13 @@
       </c>
       <c r="E5" s="70">
         <f ca="1">IF(FatCTL[[#This Row],[Saldo em PF]]=0,E4,E4+1)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="71">
         <f ca="1">IF(FatCTL[[#This Row],[Número OS]]="","",IF(FatCTL[[#This Row],[0]]=E5,"",FatCTL[[#This Row],[0]]))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="68">
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($B$1)-1))+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($B$1)-1))+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($B$1)-1))+1,OSCTL[],2,FALSE),""))</f>
@@ -4298,7 +4301,7 @@
       </c>
       <c r="E6" s="70">
         <f ca="1">IF(FatCTL[[#This Row],[Saldo em PF]]=0,E5,E5+1)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -4320,7 +4323,7 @@
       </c>
       <c r="E7" s="70">
         <f ca="1">IF(FatCTL[[#This Row],[Saldo em PF]]=0,E6,E6+1)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -4342,7 +4345,7 @@
       </c>
       <c r="E8" s="70">
         <f ca="1">IF(FatCTL[[#This Row],[Saldo em PF]]=0,E7,E7+1)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -4364,13 +4367,13 @@
       </c>
       <c r="E9" s="70">
         <f ca="1">IF(FatCTL[[#This Row],[Saldo em PF]]=0,E8,E8+1)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="71">
         <f ca="1">IF(FatCTL[[#This Row],[Número OS]]="","",IF(FatCTL[[#This Row],[0]]=E9,"",FatCTL[[#This Row],[0]]))</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="68">
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($B$1)-1))+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($B$1)-1))+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($B$1)-1))+1,OSCTL[],2,FALSE),""))</f>
@@ -4386,7 +4389,7 @@
       </c>
       <c r="E10" s="70">
         <f ca="1">IF(FatCTL[[#This Row],[Saldo em PF]]=0,E9,E9+1)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -4408,7 +4411,7 @@
       </c>
       <c r="E11" s="70">
         <f ca="1">IF(FatCTL[[#This Row],[Saldo em PF]]=0,E10,E10+1)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -4430,7 +4433,7 @@
       </c>
       <c r="E12" s="70">
         <f ca="1">IF(FatCTL[[#This Row],[Saldo em PF]]=0,E11,E11+1)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -4452,7 +4455,7 @@
       </c>
       <c r="E13" s="70">
         <f ca="1">IF(FatCTL[[#This Row],[Saldo em PF]]=0,E12,E12+1)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -4474,7 +4477,7 @@
       </c>
       <c r="E14" s="70">
         <f ca="1">IF(FatCTL[[#This Row],[Saldo em PF]]=0,E13,E13+1)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -4496,7 +4499,7 @@
       </c>
       <c r="E15" s="70">
         <f ca="1">IF(FatCTL[[#This Row],[Saldo em PF]]=0,E14,E14+1)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -4509,6 +4512,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Planilha12"/>
   <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4615,13 +4619,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Planilha2"/>
   <dimension ref="A1:Y15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4:C10"/>
+      <selection pane="bottomRight" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4730,7 +4735,7 @@
         <v>4721</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>211</v>
       </c>
       <c r="C2" s="50">
         <v>42628</v>
@@ -5337,9 +5342,6 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="Q2" calculatedColumn="1"/>
-  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -5348,16 +5350,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Planilha3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AG154"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="I5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="J12" sqref="J12"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:AG49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5392,7 +5394,7 @@
       </c>
       <c r="D1" s="59"/>
       <c r="E1" s="62" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F1" s="59"/>
       <c r="G1" s="59"/>
@@ -5522,7 +5524,7 @@
       </c>
       <c r="C4" s="78">
         <f ca="1">SUM(C5:C154)</f>
-        <v>602.19999999999993</v>
+        <v>439.6</v>
       </c>
       <c r="D4" s="67"/>
       <c r="E4" s="27"/>
@@ -5544,7 +5546,7 @@
       </c>
       <c r="B5" s="113" t="str">
         <f>IF(A5="","",VLOOKUP(A5,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
-        <v>Recebida</v>
+        <v>Recebida_</v>
       </c>
       <c r="C5" s="113"/>
       <c r="D5" s="52" t="str">
@@ -5606,11 +5608,11 @@
       </c>
       <c r="D6" s="81">
         <f ca="1">IF(E6="","",ROUND(IF($P7="",$P6,$P7)*E6,1))</f>
-        <v>216.8</v>
+        <v>0</v>
       </c>
       <c r="E6" s="87">
         <f ca="1">IF(A5="","",IF(D9&lt;0,0,IF(B5="Recebida",0.8,IF(B5="Aceita",0.2,0))))</f>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="F6" s="34">
         <f>IF(A5="","",VLOOKUP(A5,OSS[],MATCH("Abertura da OS",OSS[#Headers],0),FALSE))</f>
@@ -5935,7 +5937,7 @@
       </c>
       <c r="C9" s="88">
         <f ca="1">IF(A5="","",IF(D9&lt;0,D9,IF(D6=0,0,IF(D6&gt;D9,D6-D9,D6))))</f>
-        <v>162.60000000000002</v>
+        <v>0</v>
       </c>
       <c r="D9" s="81">
         <f ca="1">IF(P6="","",IF($P7="",$P6,$P7)+IF(D8="",0,D8)-IF(D7="",0,D7))</f>
@@ -18186,6 +18188,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Planilha4"/>
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18366,10 +18369,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Planilha5"/>
   <dimension ref="A1:AG15"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:O1"/>
+    <sheetView showGridLines="0" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18977,10 +18981,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L14"/>
+  <sheetPr codeName="Planilha6"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection sqref="A1:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19059,9 +19064,6 @@
       <c r="H3" s="104" t="s">
         <v>177</v>
       </c>
-      <c r="K3" t="s">
-        <v>210</v>
-      </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="117" t="s">
@@ -19092,24 +19094,18 @@
         <v>0</v>
       </c>
       <c r="F5" s="95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" s="96">
-        <v>27000</v>
+        <v>29983.58</v>
       </c>
       <c r="H5" s="97">
         <f>G5*F5</f>
-        <v>27000</v>
+        <v>0</v>
       </c>
       <c r="J5" s="110"/>
-      <c r="K5" s="110">
-        <f>G5*$J$13</f>
-        <v>29983.586384505019</v>
-      </c>
-      <c r="L5" s="110">
-        <f>F5*K5</f>
-        <v>29983.586384505019</v>
-      </c>
+      <c r="K5" s="110"/>
+      <c r="L5" s="110"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="117" t="s">
@@ -19140,27 +19136,22 @@
         <v>9500</v>
       </c>
       <c r="E7" s="95">
-        <v>0</v>
+        <v>216.8</v>
       </c>
       <c r="F7" s="95">
-        <v>9500</v>
+        <f ca="1">Faturamento!J2</f>
+        <v>439.6</v>
       </c>
       <c r="G7" s="96">
-        <v>630</v>
+        <v>699.62</v>
       </c>
       <c r="H7" s="97">
-        <f>G7*F7</f>
-        <v>5985000</v>
+        <f ca="1">G7*F7</f>
+        <v>307552.95199999999</v>
       </c>
       <c r="J7" s="110"/>
-      <c r="K7" s="110">
-        <f>G7*$J$13</f>
-        <v>699.61701563845043</v>
-      </c>
-      <c r="L7" s="110">
-        <f>F7*K7</f>
-        <v>6646361.6485652793</v>
-      </c>
+      <c r="K7" s="110"/>
+      <c r="L7" s="110"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="93" t="s">
@@ -19179,24 +19170,18 @@
         <v>0</v>
       </c>
       <c r="F8" s="95">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="G8" s="96">
-        <v>300</v>
+        <v>333.15</v>
       </c>
       <c r="H8" s="97">
         <f>G8*F8</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="J8" s="110"/>
-      <c r="K8" s="110">
-        <f>G8*$J$13</f>
-        <v>333.15095982783356</v>
-      </c>
-      <c r="L8" s="110">
-        <f>F8*K8</f>
-        <v>666301.91965566715</v>
-      </c>
+      <c r="K8" s="110"/>
+      <c r="L8" s="110"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="117" t="s">
@@ -19230,24 +19215,18 @@
         <v>0</v>
       </c>
       <c r="F10" s="95">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="G10" s="96">
-        <v>500</v>
+        <v>555.25</v>
       </c>
       <c r="H10" s="97">
         <f>G10*F10</f>
-        <v>250000</v>
+        <v>0</v>
       </c>
       <c r="J10" s="110"/>
-      <c r="K10" s="110">
-        <f>G10*$J$13</f>
-        <v>555.25159971305595</v>
-      </c>
-      <c r="L10" s="110">
-        <f>F10*K10</f>
-        <v>277625.799856528</v>
-      </c>
+      <c r="K10" s="110"/>
+      <c r="L10" s="110"/>
     </row>
     <row r="11" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="98" t="s">
@@ -19266,24 +19245,18 @@
         <v>0</v>
       </c>
       <c r="F11" s="95">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="G11" s="96">
-        <v>180</v>
+        <v>199.89</v>
       </c>
       <c r="H11" s="97">
         <f>G11*F11</f>
-        <v>108000</v>
+        <v>0</v>
       </c>
       <c r="J11" s="110"/>
-      <c r="K11" s="110">
-        <f>G11*$J$13</f>
-        <v>199.89057589670014</v>
-      </c>
-      <c r="L11" s="110">
-        <f>F11*K11</f>
-        <v>119934.34553802009</v>
-      </c>
+      <c r="K11" s="110"/>
+      <c r="L11" s="110"/>
     </row>
     <row r="12" spans="1:12" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="120" t="s">
@@ -19296,29 +19269,14 @@
       <c r="F12" s="121"/>
       <c r="G12" s="122"/>
       <c r="H12" s="100">
-        <f>SUM(H5:H11)</f>
-        <v>6970000</v>
-      </c>
-      <c r="J12" s="110">
-        <v>7740207.2999999998</v>
-      </c>
+        <f ca="1">SUM(H5:H11)</f>
+        <v>307552.95199999999</v>
+      </c>
+      <c r="J12" s="110"/>
       <c r="K12" s="110"/>
-      <c r="L12" s="110">
-        <f>SUM(L5:L11)</f>
-        <v>7740207.2999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="J13">
-        <f>J12/H12</f>
-        <v>1.1105031994261119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J14">
-        <v>1.1105031999999999</v>
-      </c>
-    </row>
+      <c r="L12" s="110"/>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:H1"/>
@@ -19333,10 +19291,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Planilha7"/>
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection sqref="A1:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19385,12 +19344,12 @@
       </c>
       <c r="J2" s="78">
         <f ca="1">SUM(Faturamento[PF a Faturar])</f>
-        <v>602.19999999999993</v>
+        <v>439.6</v>
       </c>
       <c r="K2" s="78"/>
       <c r="L2" s="73">
         <f ca="1">SUM(Faturamento[Valor a Faturar])</f>
-        <v>379386</v>
+        <v>307552.95199999999</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -19438,7 +19397,7 @@
       </c>
       <c r="B4" s="68">
         <f ca="1">IFERROR(VLOOKUP(ROW()-ROW($A$3),FatCTL[],2,FALSE),"")</f>
-        <v>4721</v>
+        <v>4757</v>
       </c>
       <c r="C4" s="69" t="str">
         <f ca="1">IF(B4="","",VLOOKUP(B4,OSS[],MATCH("Tipo",OSS[#Headers],0),FALSE))</f>
@@ -19450,7 +19409,7 @@
       </c>
       <c r="E4" s="85">
         <f ca="1">IF(Faturamento[[#This Row],[Número OS]]="","",IF(VLOOKUP(Faturamento[[#This Row],[Número OS]],OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="",VLOOKUP(Faturamento[[#This Row],[Número OS]],OSS[],MATCH("PF Previsto",OSS[#Headers],0),FALSE),VLOOKUP(Faturamento[[#This Row],[Número OS]],OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)))</f>
-        <v>271</v>
+        <v>94</v>
       </c>
       <c r="F4" s="84">
         <f ca="1">IF(B4="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B4,Mensal!$A$5:$A$154,0)+1,5)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B4,Mensal!$A$5:$A$154,0)+1,5)))</f>
@@ -19458,7 +19417,7 @@
       </c>
       <c r="G4" s="77">
         <f ca="1">IF(Faturamento[[#This Row],[Número OS]]="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(Faturamento[[#This Row],[Número OS]],Mensal!$A$5:$A$154,0)+1,4)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(Faturamento[[#This Row],[Número OS]],Mensal!$A$5:$A$154,0)+1,4)))</f>
-        <v>216.8</v>
+        <v>75.2</v>
       </c>
       <c r="H4" s="77">
         <f ca="1">IF(B4="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B4,Mensal!$A$5:$A$154,0)+3,4)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B4,Mensal!$A$5:$A$154,0)+3,4)))</f>
@@ -19466,19 +19425,19 @@
       </c>
       <c r="I4" s="77">
         <f ca="1">IF(Faturamento[[#This Row],[Número OS]]="","",IF(VLOOKUP(Faturamento[[#This Row],[Número OS]],OSS[],MATCH("PF Pago",OSS[#Headers],0),FALSE)="",0,VLOOKUP(Faturamento[[#This Row],[Número OS]],OSS[],MATCH("PF Pago",OSS[#Headers],0),FALSE)))</f>
-        <v>216.8</v>
+        <v>0</v>
       </c>
       <c r="J4" s="77">
         <f ca="1">IF(B4="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B4,Mensal!$A$5:$A$154,0)+4,3)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B4,Mensal!$A$5:$A$154,0)+4,3)))</f>
-        <v>162.60000000000002</v>
+        <v>75.2</v>
       </c>
       <c r="K4" s="72">
         <f ca="1">IF(Faturamento[[#This Row],[Número OS]]="","",VLOOKUP(Faturamento[[#This Row],[Tipo da OS]],TipoOS[],2,FALSE))</f>
-        <v>630</v>
+        <v>699.62</v>
       </c>
       <c r="L4" s="72">
         <f ca="1">IF(B4="","",J4*Faturamento[[#This Row],[Valor Unitario]])</f>
-        <v>102438.00000000001</v>
+        <v>52611.423999999999</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -19488,7 +19447,7 @@
       </c>
       <c r="B5" s="68">
         <f ca="1">IFERROR(VLOOKUP(ROW()-ROW($A$3),FatCTL[],2,FALSE),"")</f>
-        <v>4757</v>
+        <v>4776</v>
       </c>
       <c r="C5" s="69" t="str">
         <f ca="1">IF(B5="","",VLOOKUP(B5,OSS[],MATCH("Tipo",OSS[#Headers],0),FALSE))</f>
@@ -19500,7 +19459,7 @@
       </c>
       <c r="E5" s="85">
         <f ca="1">IF(Faturamento[[#This Row],[Número OS]]="","",IF(VLOOKUP(Faturamento[[#This Row],[Número OS]],OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="",VLOOKUP(Faturamento[[#This Row],[Número OS]],OSS[],MATCH("PF Previsto",OSS[#Headers],0),FALSE),VLOOKUP(Faturamento[[#This Row],[Número OS]],OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)))</f>
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="F5" s="84">
         <f ca="1">IF(B5="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B5,Mensal!$A$5:$A$154,0)+1,5)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B5,Mensal!$A$5:$A$154,0)+1,5)))</f>
@@ -19508,7 +19467,7 @@
       </c>
       <c r="G5" s="77">
         <f ca="1">IF(Faturamento[[#This Row],[Número OS]]="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(Faturamento[[#This Row],[Número OS]],Mensal!$A$5:$A$154,0)+1,4)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(Faturamento[[#This Row],[Número OS]],Mensal!$A$5:$A$154,0)+1,4)))</f>
-        <v>75.2</v>
+        <v>83.2</v>
       </c>
       <c r="H5" s="77">
         <f ca="1">IF(B5="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B5,Mensal!$A$5:$A$154,0)+3,4)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B5,Mensal!$A$5:$A$154,0)+3,4)))</f>
@@ -19520,15 +19479,15 @@
       </c>
       <c r="J5" s="77">
         <f ca="1">IF(B5="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B5,Mensal!$A$5:$A$154,0)+4,3)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B5,Mensal!$A$5:$A$154,0)+4,3)))</f>
-        <v>75.2</v>
+        <v>83.2</v>
       </c>
       <c r="K5" s="72">
         <f ca="1">IF(Faturamento[[#This Row],[Número OS]]="","",VLOOKUP(Faturamento[[#This Row],[Tipo da OS]],TipoOS[],2,FALSE))</f>
-        <v>630</v>
+        <v>699.62</v>
       </c>
       <c r="L5" s="72">
         <f ca="1">IF(B5="","",J5*Faturamento[[#This Row],[Valor Unitario]])</f>
-        <v>47376</v>
+        <v>58208.384000000005</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -19538,7 +19497,7 @@
       </c>
       <c r="B6" s="68">
         <f ca="1">IFERROR(VLOOKUP(ROW()-ROW($A$3),FatCTL[],2,FALSE),"")</f>
-        <v>4776</v>
+        <v>4777</v>
       </c>
       <c r="C6" s="69" t="str">
         <f ca="1">IF(B6="","",VLOOKUP(B6,OSS[],MATCH("Tipo",OSS[#Headers],0),FALSE))</f>
@@ -19550,7 +19509,7 @@
       </c>
       <c r="E6" s="85">
         <f ca="1">IF(Faturamento[[#This Row],[Número OS]]="","",IF(VLOOKUP(Faturamento[[#This Row],[Número OS]],OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="",VLOOKUP(Faturamento[[#This Row],[Número OS]],OSS[],MATCH("PF Previsto",OSS[#Headers],0),FALSE),VLOOKUP(Faturamento[[#This Row],[Número OS]],OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)))</f>
-        <v>104</v>
+        <v>168.5</v>
       </c>
       <c r="F6" s="84">
         <f ca="1">IF(B6="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B6,Mensal!$A$5:$A$154,0)+1,5)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B6,Mensal!$A$5:$A$154,0)+1,5)))</f>
@@ -19558,7 +19517,7 @@
       </c>
       <c r="G6" s="77">
         <f ca="1">IF(Faturamento[[#This Row],[Número OS]]="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(Faturamento[[#This Row],[Número OS]],Mensal!$A$5:$A$154,0)+1,4)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(Faturamento[[#This Row],[Número OS]],Mensal!$A$5:$A$154,0)+1,4)))</f>
-        <v>83.2</v>
+        <v>134.80000000000001</v>
       </c>
       <c r="H6" s="77">
         <f ca="1">IF(B6="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B6,Mensal!$A$5:$A$154,0)+3,4)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B6,Mensal!$A$5:$A$154,0)+3,4)))</f>
@@ -19570,15 +19529,15 @@
       </c>
       <c r="J6" s="77">
         <f ca="1">IF(B6="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B6,Mensal!$A$5:$A$154,0)+4,3)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B6,Mensal!$A$5:$A$154,0)+4,3)))</f>
-        <v>83.2</v>
+        <v>134.80000000000001</v>
       </c>
       <c r="K6" s="72">
         <f ca="1">IF(Faturamento[[#This Row],[Número OS]]="","",VLOOKUP(Faturamento[[#This Row],[Tipo da OS]],TipoOS[],2,FALSE))</f>
-        <v>630</v>
+        <v>699.62</v>
       </c>
       <c r="L6" s="72">
         <f ca="1">IF(B6="","",J6*Faturamento[[#This Row],[Valor Unitario]])</f>
-        <v>52416</v>
+        <v>94308.776000000013</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -19588,7 +19547,7 @@
       </c>
       <c r="B7" s="68">
         <f ca="1">IFERROR(VLOOKUP(ROW()-ROW($A$3),FatCTL[],2,FALSE),"")</f>
-        <v>4777</v>
+        <v>4782</v>
       </c>
       <c r="C7" s="69" t="str">
         <f ca="1">IF(B7="","",VLOOKUP(B7,OSS[],MATCH("Tipo",OSS[#Headers],0),FALSE))</f>
@@ -19600,7 +19559,7 @@
       </c>
       <c r="E7" s="85">
         <f ca="1">IF(Faturamento[[#This Row],[Número OS]]="","",IF(VLOOKUP(Faturamento[[#This Row],[Número OS]],OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="",VLOOKUP(Faturamento[[#This Row],[Número OS]],OSS[],MATCH("PF Previsto",OSS[#Headers],0),FALSE),VLOOKUP(Faturamento[[#This Row],[Número OS]],OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)))</f>
-        <v>168.5</v>
+        <v>160</v>
       </c>
       <c r="F7" s="84">
         <f ca="1">IF(B7="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B7,Mensal!$A$5:$A$154,0)+1,5)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B7,Mensal!$A$5:$A$154,0)+1,5)))</f>
@@ -19608,7 +19567,7 @@
       </c>
       <c r="G7" s="77">
         <f ca="1">IF(Faturamento[[#This Row],[Número OS]]="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(Faturamento[[#This Row],[Número OS]],Mensal!$A$5:$A$154,0)+1,4)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(Faturamento[[#This Row],[Número OS]],Mensal!$A$5:$A$154,0)+1,4)))</f>
-        <v>134.80000000000001</v>
+        <v>128</v>
       </c>
       <c r="H7" s="77">
         <f ca="1">IF(B7="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B7,Mensal!$A$5:$A$154,0)+3,4)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B7,Mensal!$A$5:$A$154,0)+3,4)))</f>
@@ -19620,15 +19579,15 @@
       </c>
       <c r="J7" s="77">
         <f ca="1">IF(B7="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B7,Mensal!$A$5:$A$154,0)+4,3)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B7,Mensal!$A$5:$A$154,0)+4,3)))</f>
-        <v>134.80000000000001</v>
+        <v>128</v>
       </c>
       <c r="K7" s="72">
         <f ca="1">IF(Faturamento[[#This Row],[Número OS]]="","",VLOOKUP(Faturamento[[#This Row],[Tipo da OS]],TipoOS[],2,FALSE))</f>
-        <v>630</v>
+        <v>699.62</v>
       </c>
       <c r="L7" s="72">
         <f ca="1">IF(B7="","",J7*Faturamento[[#This Row],[Valor Unitario]])</f>
-        <v>84924</v>
+        <v>89551.360000000001</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -19638,7 +19597,7 @@
       </c>
       <c r="B8" s="68">
         <f ca="1">IFERROR(VLOOKUP(ROW()-ROW($A$3),FatCTL[],2,FALSE),"")</f>
-        <v>4782</v>
+        <v>4810</v>
       </c>
       <c r="C8" s="69" t="str">
         <f ca="1">IF(B8="","",VLOOKUP(B8,OSS[],MATCH("Tipo",OSS[#Headers],0),FALSE))</f>
@@ -19650,7 +19609,7 @@
       </c>
       <c r="E8" s="85">
         <f ca="1">IF(Faturamento[[#This Row],[Número OS]]="","",IF(VLOOKUP(Faturamento[[#This Row],[Número OS]],OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="",VLOOKUP(Faturamento[[#This Row],[Número OS]],OSS[],MATCH("PF Previsto",OSS[#Headers],0),FALSE),VLOOKUP(Faturamento[[#This Row],[Número OS]],OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)))</f>
-        <v>160</v>
+        <v>23</v>
       </c>
       <c r="F8" s="84">
         <f ca="1">IF(B8="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B8,Mensal!$A$5:$A$154,0)+1,5)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B8,Mensal!$A$5:$A$154,0)+1,5)))</f>
@@ -19658,7 +19617,7 @@
       </c>
       <c r="G8" s="77">
         <f ca="1">IF(Faturamento[[#This Row],[Número OS]]="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(Faturamento[[#This Row],[Número OS]],Mensal!$A$5:$A$154,0)+1,4)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(Faturamento[[#This Row],[Número OS]],Mensal!$A$5:$A$154,0)+1,4)))</f>
-        <v>128</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="H8" s="77">
         <f ca="1">IF(B8="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B8,Mensal!$A$5:$A$154,0)+3,4)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B8,Mensal!$A$5:$A$154,0)+3,4)))</f>
@@ -19670,65 +19629,65 @@
       </c>
       <c r="J8" s="77">
         <f ca="1">IF(B8="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B8,Mensal!$A$5:$A$154,0)+4,3)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B8,Mensal!$A$5:$A$154,0)+4,3)))</f>
-        <v>128</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="K8" s="72">
         <f ca="1">IF(Faturamento[[#This Row],[Número OS]]="","",VLOOKUP(Faturamento[[#This Row],[Tipo da OS]],TipoOS[],2,FALSE))</f>
-        <v>630</v>
+        <v>699.62</v>
       </c>
       <c r="L8" s="72">
         <f ca="1">IF(B8="","",J8*Faturamento[[#This Row],[Valor Unitario]])</f>
-        <v>80640</v>
+        <v>12873.008</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="71">
+      <c r="A9" s="71" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B9" s="68">
+        <v/>
+      </c>
+      <c r="B9" s="68" t="str">
         <f ca="1">IFERROR(VLOOKUP(ROW()-ROW($A$3),FatCTL[],2,FALSE),"")</f>
-        <v>4810</v>
+        <v/>
       </c>
       <c r="C9" s="69" t="str">
         <f ca="1">IF(B9="","",VLOOKUP(B9,OSS[],MATCH("Tipo",OSS[#Headers],0),FALSE))</f>
-        <v>PF Java</v>
+        <v/>
       </c>
       <c r="D9" s="83" t="str">
         <f ca="1">IF(B9="","",VLOOKUP(B9,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
-        <v>Recebida</v>
-      </c>
-      <c r="E9" s="85">
+        <v/>
+      </c>
+      <c r="E9" s="85" t="str">
         <f ca="1">IF(Faturamento[[#This Row],[Número OS]]="","",IF(VLOOKUP(Faturamento[[#This Row],[Número OS]],OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="",VLOOKUP(Faturamento[[#This Row],[Número OS]],OSS[],MATCH("PF Previsto",OSS[#Headers],0),FALSE),VLOOKUP(Faturamento[[#This Row],[Número OS]],OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)))</f>
-        <v>23</v>
-      </c>
-      <c r="F9" s="84">
+        <v/>
+      </c>
+      <c r="F9" s="84" t="str">
         <f ca="1">IF(B9="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B9,Mensal!$A$5:$A$154,0)+1,5)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B9,Mensal!$A$5:$A$154,0)+1,5)))</f>
-        <v>0.8</v>
-      </c>
-      <c r="G9" s="77">
+        <v/>
+      </c>
+      <c r="G9" s="77" t="str">
         <f ca="1">IF(Faturamento[[#This Row],[Número OS]]="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(Faturamento[[#This Row],[Número OS]],Mensal!$A$5:$A$154,0)+1,4)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(Faturamento[[#This Row],[Número OS]],Mensal!$A$5:$A$154,0)+1,4)))</f>
-        <v>18.399999999999999</v>
-      </c>
-      <c r="H9" s="77">
+        <v/>
+      </c>
+      <c r="H9" s="77" t="str">
         <f ca="1">IF(B9="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B9,Mensal!$A$5:$A$154,0)+3,4)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B9,Mensal!$A$5:$A$154,0)+3,4)))</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="77">
+        <v/>
+      </c>
+      <c r="I9" s="77" t="str">
         <f ca="1">IF(Faturamento[[#This Row],[Número OS]]="","",IF(VLOOKUP(Faturamento[[#This Row],[Número OS]],OSS[],MATCH("PF Pago",OSS[#Headers],0),FALSE)="",0,VLOOKUP(Faturamento[[#This Row],[Número OS]],OSS[],MATCH("PF Pago",OSS[#Headers],0),FALSE)))</f>
-        <v>0</v>
-      </c>
-      <c r="J9" s="77">
+        <v/>
+      </c>
+      <c r="J9" s="77" t="str">
         <f ca="1">IF(B9="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B9,Mensal!$A$5:$A$154,0)+4,3)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B9,Mensal!$A$5:$A$154,0)+4,3)))</f>
-        <v>18.399999999999999</v>
-      </c>
-      <c r="K9" s="72">
+        <v/>
+      </c>
+      <c r="K9" s="72" t="str">
         <f ca="1">IF(Faturamento[[#This Row],[Número OS]]="","",VLOOKUP(Faturamento[[#This Row],[Tipo da OS]],TipoOS[],2,FALSE))</f>
-        <v>630</v>
-      </c>
-      <c r="L9" s="72">
+        <v/>
+      </c>
+      <c r="L9" s="72" t="str">
         <f ca="1">IF(B9="","",J9*Faturamento[[#This Row],[Valor Unitario]])</f>
-        <v>11592</v>
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -20142,11 +20101,12 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Planilha8"/>
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I20" sqref="I20"/>
+      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20586,6 +20546,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Planilha9"/>
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20612,7 +20573,7 @@
       </c>
       <c r="B2" s="86">
         <f>QuadroResumo!G5</f>
-        <v>27000</v>
+        <v>29983.58</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -20621,7 +20582,7 @@
       </c>
       <c r="B3" s="86">
         <f>QuadroResumo!G7</f>
-        <v>630</v>
+        <v>699.62</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -20630,7 +20591,7 @@
       </c>
       <c r="B4" s="86">
         <f>QuadroResumo!G8</f>
-        <v>300</v>
+        <v>333.15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -20639,7 +20600,7 @@
       </c>
       <c r="B5" s="86">
         <f>QuadroResumo!G10</f>
-        <v>500</v>
+        <v>555.25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -20648,7 +20609,7 @@
       </c>
       <c r="B6" s="86">
         <f>QuadroResumo!G11</f>
-        <v>180</v>
+        <v>199.89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>